<commit_message>
copy blank rows to output wb
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/expected/writerSpec.xlsx
+++ b/src/test/resources/excel/expected/writerSpec.xlsx
@@ -49,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -108,8 +109,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -136,9 +141,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>693720</xdr:colOff>
+      <xdr:colOff>693000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -151,8 +156,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2854440" y="270000"/>
-          <a:ext cx="1902960" cy="963720"/>
+          <a:off x="2862000" y="270000"/>
+          <a:ext cx="1907640" cy="963000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -175,40 +180,40 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1.45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1.573</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>2.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sequential Repeated Rows - Blank Row Fix (#22)
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/expected/writerSpec.xlsx
+++ b/src/test/resources/excel/expected/writerSpec.xlsx
@@ -49,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -108,8 +109,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -136,9 +141,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>693720</xdr:colOff>
+      <xdr:colOff>693000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -151,8 +156,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2854440" y="270000"/>
-          <a:ext cx="1902960" cy="963720"/>
+          <a:off x="2862000" y="270000"/>
+          <a:ext cx="1907640" cy="963000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -175,40 +180,40 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1.45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1.573</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>2.5</v>
       </c>
     </row>

</xml_diff>